<commit_message>
adding a new file
</commit_message>
<xml_diff>
--- a/user-guide/OLTCO <> i4T Pilot-UAC.xlsx
+++ b/user-guide/OLTCO <> i4T Pilot-UAC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shehan/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04A58452-0491-A640-9618-3212B4D38F8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D92FAF3-8E03-B446-AC63-B2C4F5E8DCEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="36000" windowHeight="22620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,21 +46,9 @@
     <t>Assigning an individual employee to a visit</t>
   </si>
   <si>
-    <t>Assigning a team to a visit</t>
-  </si>
-  <si>
     <t>Dispatching visits</t>
   </si>
   <si>
-    <t>Viewing upcoming and past visits</t>
-  </si>
-  <si>
-    <t>Site visit notifications and reminders</t>
-  </si>
-  <si>
-    <t>Route tracking link shared with the customer via WhatsApp</t>
-  </si>
-  <si>
     <t>Rescheduling site visits</t>
   </si>
   <si>
@@ -68,9 +56,6 @@
   </si>
   <si>
     <t>Field App Operations — i4T Business Lite</t>
-  </si>
-  <si>
-    <t>Download the "i4T Business Lite" app from Apple Store / Google Play Store</t>
   </si>
   <si>
     <t>User login and first-run experience</t>
@@ -209,9 +194,6 @@
     <t>Manually mark invoice as “Paid” if payment is received by a bank transfer</t>
   </si>
   <si>
-    <t xml:space="preserve">Upon submission the invoice will be sync with XERO automatically </t>
-  </si>
-  <si>
     <t>Material Order</t>
   </si>
   <si>
@@ -240,9 +222,6 @@
   </si>
   <si>
     <t>Reschedule the material delivery date within the purchase/material order module</t>
-  </si>
-  <si>
-    <t>Upon rescheduling, system will automatically update installation schedules to reflect the new delivery date and alert all the stakeholders</t>
   </si>
   <si>
     <t>Installation</t>
@@ -391,14 +370,35 @@
     </r>
   </si>
   <si>
-    <t>Setup Reminders - Will be done by i4T</t>
+    <t>Receive the new site visit and check the details</t>
+  </si>
+  <si>
+    <t>Route tracking link shared with the customer via WhatsApp (Coming Soon)</t>
+  </si>
+  <si>
+    <t>Upon submission the invoice will be sync with XERO automatically (Coming Soon)</t>
+  </si>
+  <si>
+    <t>Upon rescheduling, system will automatically update installation schedules to reflect the new delivery date and alert all the stakeholders (Coming Soon)</t>
+  </si>
+  <si>
+    <t>Setup Reminders - Will be done by i4T (Coming Soon)</t>
+  </si>
+  <si>
+    <t>Viewing upcoming and past visits using the calendar (Diary)</t>
+  </si>
+  <si>
+    <t>Download the "i4T Business Lite" app from Apple Store / Google Play Store (Coming Soon)</t>
+  </si>
+  <si>
+    <t>Download the Test App (Follow the Userguide)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -425,21 +425,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color rgb="FF999999"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FFB7B7B7"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
@@ -471,6 +459,41 @@
     <font>
       <sz val="14"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF999999"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFB7B7B7"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="0" tint="-0.499984740745262"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -517,7 +540,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -526,36 +549,21 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <extLst>
         <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
@@ -563,9 +571,27 @@
         </ext>
       </extLst>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -804,8 +830,8 @@
   <dimension ref="A1:D138"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -817,7 +843,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -831,295 +857,290 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-    </row>
-    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C3" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" s="3"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+    </row>
+    <row r="3" spans="1:4" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" s="11" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C4" s="18" t="b">
+        <v>5</v>
+      </c>
+      <c r="B4" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C5" s="18" t="b">
+        <v>6</v>
+      </c>
+      <c r="B5" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C6" s="18" t="b">
+        <v>7</v>
+      </c>
+      <c r="B6" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C7" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A8" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="B8" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C8" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A9" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C7" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="D7" s="3"/>
-    </row>
-    <row r="8" spans="1:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C8" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="1:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C9" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="1:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
+      <c r="B10" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C10" s="11" t="b">
+        <v>0</v>
+      </c>
       <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C11" s="18" t="b">
+        <v>10</v>
+      </c>
+      <c r="B11" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C11" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C12" s="18" t="b">
-        <v>0</v>
-      </c>
+      <c r="A12" s="4"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="A13" s="5"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
+    <row r="13" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+    </row>
+    <row r="14" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A14" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C15" s="18" t="b">
+      <c r="A15" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="B15" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C15" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C16" s="18" t="b">
+        <v>12</v>
+      </c>
+      <c r="B16" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C16" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C17" s="18" t="b">
+        <v>13</v>
+      </c>
+      <c r="B17" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C17" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C18" s="18" t="b">
+        <v>14</v>
+      </c>
+      <c r="B18" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C18" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D18" s="3"/>
     </row>
     <row r="19" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C19" s="18" t="b">
+        <v>15</v>
+      </c>
+      <c r="B19" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C19" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D19" s="3"/>
     </row>
     <row r="20" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C20" s="18" t="b">
+        <v>16</v>
+      </c>
+      <c r="B20" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C20" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D20" s="3"/>
     </row>
     <row r="21" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C21" s="18" t="b">
+        <v>17</v>
+      </c>
+      <c r="B21" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C21" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D21" s="3"/>
     </row>
     <row r="22" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C22" s="18" t="b">
+        <v>18</v>
+      </c>
+      <c r="B22" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C22" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D22" s="3"/>
     </row>
     <row r="23" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C23" s="18" t="b">
+        <v>19</v>
+      </c>
+      <c r="B23" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C23" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D23" s="3"/>
     </row>
     <row r="24" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C24" s="18" t="b">
+        <v>20</v>
+      </c>
+      <c r="B24" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C24" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D24" s="3"/>
     </row>
     <row r="25" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C25" s="18" t="b">
+        <v>21</v>
+      </c>
+      <c r="B25" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C25" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D25" s="3"/>
     </row>
     <row r="26" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C26" s="18" t="b">
+        <v>22</v>
+      </c>
+      <c r="B26" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C26" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D26" s="3"/>
     </row>
     <row r="27" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C27" s="18" t="b">
+        <v>23</v>
+      </c>
+      <c r="B27" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C27" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D27" s="3"/>
@@ -1132,140 +1153,140 @@
     </row>
     <row r="29" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
+        <v>24</v>
+      </c>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
     </row>
     <row r="30" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C30" s="18" t="b">
+        <v>25</v>
+      </c>
+      <c r="B30" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C30" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D30" s="3"/>
     </row>
     <row r="31" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B31" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C31" s="18" t="b">
+        <v>26</v>
+      </c>
+      <c r="B31" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C31" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D31" s="3"/>
     </row>
     <row r="32" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B32" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C32" s="18" t="b">
+        <v>27</v>
+      </c>
+      <c r="B32" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C32" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D32" s="3"/>
     </row>
     <row r="33" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B33" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C33" s="18" t="b">
+        <v>28</v>
+      </c>
+      <c r="B33" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C33" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D33" s="3"/>
     </row>
     <row r="34" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B34" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C34" s="18" t="b">
+        <v>29</v>
+      </c>
+      <c r="B34" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C34" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D34" s="3"/>
     </row>
     <row r="35" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B35" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C35" s="18" t="b">
+        <v>30</v>
+      </c>
+      <c r="B35" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C35" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D35" s="3"/>
     </row>
     <row r="36" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B36" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C36" s="18" t="b">
+        <v>31</v>
+      </c>
+      <c r="B36" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C36" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D36" s="3"/>
     </row>
     <row r="37" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B37" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C37" s="18" t="b">
+        <v>32</v>
+      </c>
+      <c r="B37" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C37" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D37" s="3"/>
     </row>
     <row r="38" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B38" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C38" s="18" t="b">
+        <v>33</v>
+      </c>
+      <c r="B38" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C38" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D38" s="3"/>
     </row>
     <row r="39" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B39" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C39" s="18" t="b">
+        <v>34</v>
+      </c>
+      <c r="B39" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C39" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D39" s="3"/>
     </row>
     <row r="40" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B40" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C40" s="18" t="b">
+        <v>35</v>
+      </c>
+      <c r="B40" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C40" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D40" s="3"/>
@@ -1278,93 +1299,93 @@
     </row>
     <row r="42" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B42" s="6"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
+        <v>36</v>
+      </c>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
     </row>
     <row r="43" spans="1:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="A43" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B43" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C43" s="18" t="b">
+      <c r="A43" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B43" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C43" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D43" s="3"/>
     </row>
     <row r="44" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B44" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C44" s="18" t="b">
+        <v>38</v>
+      </c>
+      <c r="B44" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C44" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D44" s="3"/>
     </row>
     <row r="45" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B45" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C45" s="18" t="b">
+        <v>39</v>
+      </c>
+      <c r="B45" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C45" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D45" s="3"/>
     </row>
     <row r="46" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B46" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C46" s="18" t="b">
+        <v>40</v>
+      </c>
+      <c r="B46" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C46" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D46" s="3"/>
     </row>
     <row r="47" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B47" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C47" s="18" t="b">
+        <v>41</v>
+      </c>
+      <c r="B47" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C47" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D47" s="3"/>
     </row>
     <row r="48" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B48" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C48" s="18" t="b">
+        <v>42</v>
+      </c>
+      <c r="B48" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C48" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D48" s="3"/>
     </row>
     <row r="49" spans="1:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="A49" s="7"/>
+      <c r="A49" s="6"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
     </row>
     <row r="50" spans="1:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="A50" s="7" t="s">
-        <v>48</v>
+      <c r="A50" s="6" t="s">
+        <v>43</v>
       </c>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
@@ -1372,322 +1393,322 @@
     </row>
     <row r="51" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B51" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C51" s="18" t="b">
+        <v>44</v>
+      </c>
+      <c r="B51" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C51" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D51" s="3"/>
     </row>
     <row r="52" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B52" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C52" s="18" t="b">
+        <v>45</v>
+      </c>
+      <c r="B52" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C52" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D52" s="3"/>
     </row>
     <row r="53" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B53" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C53" s="18" t="b">
+        <v>46</v>
+      </c>
+      <c r="B53" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C53" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D53" s="3"/>
     </row>
     <row r="54" spans="1:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="A54" s="5"/>
+      <c r="A54" s="4"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
     </row>
     <row r="55" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B55" s="5"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+    </row>
+    <row r="56" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="A56" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B56" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C56" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D56" s="3"/>
+    </row>
+    <row r="57" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="A57" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B57" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C57" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D57" s="3"/>
+    </row>
+    <row r="58" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="A58" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B58" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C58" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D58" s="3"/>
+    </row>
+    <row r="59" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="A59" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B59" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C59" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D59" s="3"/>
+    </row>
+    <row r="60" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="A60" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B55" s="6"/>
-      <c r="C55" s="6"/>
-      <c r="D55" s="6"/>
-    </row>
-    <row r="56" spans="1:4" ht="19" x14ac:dyDescent="0.2">
-      <c r="A56" s="8" t="s">
+      <c r="B60" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C60" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D60" s="3"/>
+    </row>
+    <row r="61" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="A61" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B56" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C56" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="D56" s="3"/>
-    </row>
-    <row r="57" spans="1:4" ht="19" x14ac:dyDescent="0.2">
-      <c r="A57" s="8" t="s">
+      <c r="B61" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C61" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D61" s="3"/>
+    </row>
+    <row r="62" spans="1:4" ht="38" x14ac:dyDescent="0.2">
+      <c r="A62" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B57" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C57" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="D57" s="3"/>
-    </row>
-    <row r="58" spans="1:4" ht="19" x14ac:dyDescent="0.2">
-      <c r="A58" s="8" t="s">
+      <c r="B62" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C62" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D62" s="3"/>
+    </row>
+    <row r="63" spans="1:4" ht="38" x14ac:dyDescent="0.2">
+      <c r="A63" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B58" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C58" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="D58" s="3"/>
-    </row>
-    <row r="59" spans="1:4" ht="19" x14ac:dyDescent="0.2">
-      <c r="A59" s="8" t="s">
+      <c r="B63" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C63" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D63" s="3"/>
+    </row>
+    <row r="64" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="A64" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B59" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C59" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="D59" s="3"/>
-    </row>
-    <row r="60" spans="1:4" ht="19" x14ac:dyDescent="0.2">
-      <c r="A60" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="B60" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C60" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="D60" s="3"/>
-    </row>
-    <row r="61" spans="1:4" ht="19" x14ac:dyDescent="0.2">
-      <c r="A61" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="B61" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C61" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="D61" s="3"/>
-    </row>
-    <row r="62" spans="1:4" ht="38" x14ac:dyDescent="0.2">
-      <c r="A62" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="B62" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C62" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="D62" s="3"/>
-    </row>
-    <row r="63" spans="1:4" ht="38" x14ac:dyDescent="0.2">
-      <c r="A63" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="B63" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C63" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="D63" s="3"/>
-    </row>
-    <row r="64" spans="1:4" ht="19" x14ac:dyDescent="0.2">
-      <c r="A64" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="B64" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C64" s="18" t="b">
+      <c r="B64" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C64" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D64" s="3"/>
     </row>
     <row r="65" spans="1:4" ht="19" x14ac:dyDescent="0.2">
-      <c r="A65" s="9" t="s">
-        <v>62</v>
+      <c r="A65" s="19" t="s">
+        <v>103</v>
       </c>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
     </row>
     <row r="66" spans="1:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="A66" s="5"/>
+      <c r="A66" s="4"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
     </row>
     <row r="67" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B67" s="6"/>
-      <c r="C67" s="6"/>
-      <c r="D67" s="6"/>
+        <v>57</v>
+      </c>
+      <c r="B67" s="5"/>
+      <c r="C67" s="5"/>
+      <c r="D67" s="5"/>
     </row>
     <row r="68" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B68" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C68" s="18" t="b">
+        <v>58</v>
+      </c>
+      <c r="B68" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C68" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D68" s="3"/>
     </row>
     <row r="69" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B69" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C69" s="18" t="b">
+        <v>59</v>
+      </c>
+      <c r="B69" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C69" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D69" s="3"/>
     </row>
     <row r="70" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B70" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C70" s="18" t="b">
+        <v>60</v>
+      </c>
+      <c r="B70" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C70" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D70" s="3"/>
     </row>
     <row r="71" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B71" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C71" s="18" t="b">
+        <v>61</v>
+      </c>
+      <c r="B71" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C71" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D71" s="3"/>
     </row>
     <row r="72" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B72" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C72" s="18" t="b">
+        <v>62</v>
+      </c>
+      <c r="B72" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C72" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D72" s="3"/>
     </row>
     <row r="73" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B73" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C73" s="18" t="b">
+        <v>63</v>
+      </c>
+      <c r="B73" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C73" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D73" s="3"/>
     </row>
     <row r="74" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B74" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C74" s="18" t="b">
+        <v>64</v>
+      </c>
+      <c r="B74" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C74" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D74" s="3"/>
     </row>
     <row r="75" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B75" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C75" s="18" t="b">
+        <v>65</v>
+      </c>
+      <c r="B75" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C75" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D75" s="3"/>
     </row>
     <row r="76" spans="1:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="A76" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="B76" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C76" s="18" t="b">
+      <c r="A76" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B76" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C76" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D76" s="3"/>
     </row>
     <row r="77" spans="1:4" ht="38" x14ac:dyDescent="0.2">
-      <c r="A77" s="11" t="s">
-        <v>73</v>
+      <c r="A77" s="20" t="s">
+        <v>104</v>
       </c>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
       <c r="D77" s="3"/>
     </row>
     <row r="78" spans="1:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="A78" s="5"/>
+      <c r="A78" s="4"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
       <c r="D78" s="3"/>
     </row>
     <row r="79" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A79" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B79" s="6"/>
-      <c r="C79" s="6"/>
-      <c r="D79" s="6"/>
+        <v>67</v>
+      </c>
+      <c r="B79" s="5"/>
+      <c r="C79" s="5"/>
+      <c r="D79" s="5"/>
     </row>
     <row r="80" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B80" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C80" s="18" t="b">
+        <v>68</v>
+      </c>
+      <c r="B80" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C80" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D80" s="3"/>
@@ -1696,77 +1717,77 @@
       <c r="A81" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B81" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C81" s="18" t="b">
+      <c r="B81" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C81" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D81" s="3"/>
     </row>
     <row r="82" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B82" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C82" s="18" t="b">
+        <v>69</v>
+      </c>
+      <c r="B82" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C82" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D82" s="3"/>
     </row>
     <row r="83" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B83" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C83" s="18" t="b">
+        <v>70</v>
+      </c>
+      <c r="B83" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C83" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D83" s="3"/>
     </row>
     <row r="84" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B84" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C84" s="18" t="b">
+        <v>71</v>
+      </c>
+      <c r="B84" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C84" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D84" s="3"/>
     </row>
     <row r="85" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="B85" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C85" s="18" t="b">
+        <v>72</v>
+      </c>
+      <c r="B85" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C85" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D85" s="3"/>
     </row>
     <row r="86" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B86" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C86" s="18" t="b">
+        <v>73</v>
+      </c>
+      <c r="B86" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C86" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D86" s="3"/>
     </row>
     <row r="87" spans="1:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="A87" s="4" t="s">
-        <v>12</v>
+      <c r="A87" s="18" t="s">
+        <v>102</v>
       </c>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
@@ -1774,191 +1795,191 @@
     </row>
     <row r="88" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B88" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C88" s="18" t="b">
+        <v>74</v>
+      </c>
+      <c r="B88" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C88" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D88" s="3"/>
     </row>
     <row r="89" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B89" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C89" s="18" t="b">
+        <v>75</v>
+      </c>
+      <c r="B89" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C89" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D89" s="3"/>
     </row>
     <row r="90" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B90" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C90" s="18" t="b">
+        <v>76</v>
+      </c>
+      <c r="B90" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C90" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D90" s="3"/>
     </row>
     <row r="91" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B91" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C91" s="18" t="b">
+        <v>18</v>
+      </c>
+      <c r="B91" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C91" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D91" s="3"/>
     </row>
     <row r="92" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B92" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C92" s="18" t="b">
+        <v>77</v>
+      </c>
+      <c r="B92" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C92" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D92" s="3"/>
     </row>
     <row r="93" spans="1:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="A93" s="5"/>
+      <c r="A93" s="4"/>
       <c r="B93" s="3"/>
       <c r="C93" s="3"/>
       <c r="D93" s="3"/>
     </row>
     <row r="94" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A94" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B94" s="6"/>
-      <c r="C94" s="6"/>
-      <c r="D94" s="6"/>
+        <v>78</v>
+      </c>
+      <c r="B94" s="5"/>
+      <c r="C94" s="5"/>
+      <c r="D94" s="5"/>
     </row>
     <row r="95" spans="1:4" ht="19" x14ac:dyDescent="0.2">
-      <c r="A95" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="B95" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C95" s="18" t="b">
+      <c r="A95" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B95" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C95" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D95" s="3"/>
     </row>
     <row r="96" spans="1:4" ht="19" x14ac:dyDescent="0.2">
-      <c r="A96" s="8" t="s">
+      <c r="A96" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B96" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C96" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D96" s="3"/>
+    </row>
+    <row r="97" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="A97" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B97" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C97" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D97" s="3"/>
+    </row>
+    <row r="98" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="A98" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B98" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C98" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D98" s="3"/>
+    </row>
+    <row r="99" spans="1:4" ht="38" x14ac:dyDescent="0.2">
+      <c r="A99" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B99" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C99" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D99" s="3"/>
+    </row>
+    <row r="100" spans="1:4" ht="38" x14ac:dyDescent="0.2">
+      <c r="A100" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B100" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C100" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D100" s="3"/>
+    </row>
+    <row r="101" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="A101" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B96" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C96" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="D96" s="3"/>
-    </row>
-    <row r="97" spans="1:4" ht="19" x14ac:dyDescent="0.2">
-      <c r="A97" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="B97" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C97" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="D97" s="3"/>
-    </row>
-    <row r="98" spans="1:4" ht="19" x14ac:dyDescent="0.2">
-      <c r="A98" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="B98" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C98" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="D98" s="3"/>
-    </row>
-    <row r="99" spans="1:4" ht="38" x14ac:dyDescent="0.2">
-      <c r="A99" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="B99" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C99" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="D99" s="3"/>
-    </row>
-    <row r="100" spans="1:4" ht="38" x14ac:dyDescent="0.2">
-      <c r="A100" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="B100" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C100" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="D100" s="3"/>
-    </row>
-    <row r="101" spans="1:4" ht="19" x14ac:dyDescent="0.2">
-      <c r="A101" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="B101" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C101" s="18" t="b">
+      <c r="B101" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C101" s="11" t="b">
         <v>0</v>
       </c>
       <c r="D101" s="3"/>
     </row>
     <row r="102" spans="1:4" ht="19" x14ac:dyDescent="0.2">
-      <c r="A102" s="9" t="s">
-        <v>62</v>
+      <c r="A102" s="19" t="s">
+        <v>103</v>
       </c>
       <c r="B102" s="3"/>
       <c r="C102" s="3"/>
       <c r="D102" s="3"/>
     </row>
     <row r="103" spans="1:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="A103" s="5"/>
+      <c r="A103" s="4"/>
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
       <c r="D103" s="3"/>
     </row>
     <row r="104" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A104" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B104" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="C104" s="6"/>
-      <c r="D104" s="6"/>
+        <v>81</v>
+      </c>
+      <c r="B104" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C104" s="5"/>
+      <c r="D104" s="5"/>
     </row>
     <row r="105" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B105" s="18" t="b">
+        <v>83</v>
+      </c>
+      <c r="B105" s="11" t="b">
         <v>0</v>
       </c>
       <c r="C105" s="3"/>
@@ -1966,29 +1987,29 @@
     </row>
     <row r="106" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B106" s="18" t="b">
+        <v>84</v>
+      </c>
+      <c r="B106" s="11" t="b">
         <v>0</v>
       </c>
       <c r="C106" s="3"/>
-      <c r="D106" s="13"/>
+      <c r="D106" s="10"/>
     </row>
     <row r="107" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B107" s="18" t="b">
+        <v>85</v>
+      </c>
+      <c r="B107" s="11" t="b">
         <v>0</v>
       </c>
       <c r="C107" s="3"/>
-      <c r="D107" s="13"/>
+      <c r="D107" s="10"/>
     </row>
     <row r="108" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B108" s="18" t="b">
+        <v>86</v>
+      </c>
+      <c r="B108" s="11" t="b">
         <v>0</v>
       </c>
       <c r="C108" s="3"/>
@@ -1996,9 +2017,9 @@
     </row>
     <row r="109" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B109" s="18" t="b">
+        <v>87</v>
+      </c>
+      <c r="B109" s="11" t="b">
         <v>0</v>
       </c>
       <c r="C109" s="3"/>
@@ -2006,45 +2027,45 @@
     </row>
     <row r="110" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B110" s="18" t="b">
+        <v>88</v>
+      </c>
+      <c r="B110" s="11" t="b">
         <v>0</v>
       </c>
       <c r="C110" s="3"/>
     </row>
     <row r="111" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B111" s="18" t="b">
+        <v>89</v>
+      </c>
+      <c r="B111" s="11" t="b">
         <v>0</v>
       </c>
       <c r="C111" s="3"/>
     </row>
     <row r="114" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A114" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="B114" s="17"/>
-      <c r="C114" s="17"/>
-      <c r="D114" s="17"/>
+      <c r="A114" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="B114" s="16"/>
+      <c r="C114" s="16"/>
+      <c r="D114" s="16"/>
     </row>
     <row r="117" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A117" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B117" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="C117" s="6"/>
-      <c r="D117" s="6"/>
+        <v>91</v>
+      </c>
+      <c r="B117" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C117" s="5"/>
+      <c r="D117" s="5"/>
     </row>
     <row r="118" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A118" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B118" s="18" t="b">
+        <v>92</v>
+      </c>
+      <c r="B118" s="11" t="b">
         <v>0</v>
       </c>
       <c r="C118" s="3"/>
@@ -2052,9 +2073,9 @@
     </row>
     <row r="119" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A119" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="B119" s="18" t="b">
+        <v>93</v>
+      </c>
+      <c r="B119" s="11" t="b">
         <v>0</v>
       </c>
       <c r="C119" s="3"/>
@@ -2062,9 +2083,9 @@
     </row>
     <row r="120" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A120" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B120" s="18" t="b">
+        <v>94</v>
+      </c>
+      <c r="B120" s="11" t="b">
         <v>0</v>
       </c>
       <c r="C120" s="3"/>
@@ -2072,9 +2093,9 @@
     </row>
     <row r="121" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A121" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B121" s="18" t="b">
+        <v>95</v>
+      </c>
+      <c r="B121" s="11" t="b">
         <v>0</v>
       </c>
       <c r="C121" s="3"/>
@@ -2082,9 +2103,9 @@
     </row>
     <row r="122" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A122" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B122" s="18" t="b">
+        <v>96</v>
+      </c>
+      <c r="B122" s="11" t="b">
         <v>0</v>
       </c>
       <c r="C122" s="3"/>
@@ -2092,9 +2113,9 @@
     </row>
     <row r="123" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A123" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="B123" s="18" t="b">
+        <v>97</v>
+      </c>
+      <c r="B123" s="11" t="b">
         <v>0</v>
       </c>
       <c r="C123" s="3"/>
@@ -2102,9 +2123,9 @@
     </row>
     <row r="124" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A124" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="B124" s="18" t="b">
+        <v>98</v>
+      </c>
+      <c r="B124" s="11" t="b">
         <v>0</v>
       </c>
       <c r="C124" s="3"/>
@@ -2112,9 +2133,9 @@
     </row>
     <row r="125" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A125" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="B125" s="18" t="b">
+        <v>99</v>
+      </c>
+      <c r="B125" s="11" t="b">
         <v>0</v>
       </c>
       <c r="C125" s="3"/>
@@ -2122,21 +2143,21 @@
     </row>
     <row r="126" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A126" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="B126" s="18" t="b">
+        <v>100</v>
+      </c>
+      <c r="B126" s="11" t="b">
         <v>0</v>
       </c>
       <c r="C126" s="3"/>
-      <c r="D126" s="13"/>
+      <c r="D126" s="10"/>
     </row>
     <row r="127" spans="1:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="A127" s="4" t="s">
-        <v>108</v>
+      <c r="A127" s="18" t="s">
+        <v>105</v>
       </c>
       <c r="B127" s="3"/>
       <c r="C127" s="3"/>
-      <c r="D127" s="13"/>
+      <c r="D127" s="10"/>
     </row>
     <row r="128" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="B128" s="3"/>
@@ -2199,7 +2220,7 @@
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A13:D13"/>
     <mergeCell ref="A114:D114"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>